<commit_message>
Testing and Bugfix 2
</commit_message>
<xml_diff>
--- a/res/Test Checklist.xlsx
+++ b/res/Test Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Desktop\Cycling Coursework\ECM1410-Cycling-Coursework\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9ACAA9-8420-44FA-A2CD-0626EFF29C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A401BAB-32F3-47EC-AD98-FA83680FEB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1EAC307A-8FFF-4A01-A94B-72348606857C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Function</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>Half</t>
   </si>
 </sst>
 </file>
@@ -552,7 +549,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,7 +571,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -594,6 +591,9 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -748,37 +748,40 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Testing, LocalTime is awful
</commit_message>
<xml_diff>
--- a/res/Test Checklist.xlsx
+++ b/res/Test Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Desktop\Cycling Coursework\ECM1410-Cycling-Coursework\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0E2C98-E6B9-489C-AB58-7655C0C824B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C43B56-9A05-4311-B731-5A99163B5D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1EAC307A-8FFF-4A01-A94B-72348606857C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>Function</t>
   </si>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF95829D-63CA-40D7-A9D1-5225706937C4}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,16 +746,25 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="B11" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -766,6 +775,9 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
+      <c r="B15" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -819,10 +831,16 @@
       <c r="A22" t="s">
         <v>22</v>
       </c>
+      <c r="B22" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Serialization Testing and Fixes
</commit_message>
<xml_diff>
--- a/res/Test Checklist.xlsx
+++ b/res/Test Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Desktop\Cycling Coursework\ECM1410-Cycling-Coursework\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C43B56-9A05-4311-B731-5A99163B5D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2392B79-6F89-4ABF-A2BB-ECBEF02C4F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1EAC307A-8FFF-4A01-A94B-72348606857C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
   <si>
     <t>Function</t>
   </si>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF95829D-63CA-40D7-A9D1-5225706937C4}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,6 +770,9 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
+      <c r="B14" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -877,15 +880,24 @@
       <c r="A30" t="s">
         <v>30</v>
       </c>
+      <c r="B30" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
+      <c r="B31" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>